<commit_message>
Refactored the code to ensure no flaky tests and
screenshots are added correctly
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="108">
   <si>
     <t>Runmode</t>
   </si>
@@ -311,6 +311,36 @@
   </si>
   <si>
     <t>This is an Automation Test 3</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>1996</t>
+  </si>
+  <si>
+    <t>172</t>
+  </si>
+  <si>
+    <t>65</t>
+  </si>
+  <si>
+    <t>35.3</t>
+  </si>
+  <si>
+    <t>90</t>
+  </si>
+  <si>
+    <t>120</t>
+  </si>
+  <si>
+    <t>80</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>60</t>
   </si>
 </sst>
 </file>
@@ -388,7 +418,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -417,6 +447,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -823,8 +856,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37:F39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -972,14 +1005,14 @@
       <c r="E11" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="F11" s="6">
-        <v>30</v>
+      <c r="F11" s="11" t="s">
+        <v>98</v>
       </c>
       <c r="G11" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="H11" s="6">
-        <v>1996</v>
+      <c r="H11" s="11" t="s">
+        <v>99</v>
       </c>
       <c r="I11" s="6" t="s">
         <v>73</v>
@@ -1041,14 +1074,14 @@
       <c r="E15" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="F15" s="6">
-        <v>30</v>
+      <c r="F15" s="11" t="s">
+        <v>98</v>
       </c>
       <c r="G15" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="H15" s="6">
-        <v>1996</v>
+      <c r="H15" s="11" t="s">
+        <v>99</v>
       </c>
       <c r="I15" s="6" t="s">
         <v>73</v>
@@ -1111,14 +1144,14 @@
       <c r="E19" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="F19" s="6">
-        <v>30</v>
+      <c r="F19" s="11" t="s">
+        <v>98</v>
       </c>
       <c r="G19" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="H19" s="6">
-        <v>1996</v>
+      <c r="H19" s="11" t="s">
+        <v>99</v>
       </c>
       <c r="I19" s="6" t="s">
         <v>73</v>
@@ -1171,26 +1204,26 @@
       <c r="B23" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C23" s="6">
-        <v>172</v>
-      </c>
-      <c r="D23" s="6">
-        <v>65</v>
-      </c>
-      <c r="E23" s="6">
-        <v>35.299999999999997</v>
-      </c>
-      <c r="F23" s="6">
-        <v>90</v>
-      </c>
-      <c r="G23" s="6">
-        <v>120</v>
-      </c>
-      <c r="H23" s="6">
-        <v>80</v>
-      </c>
-      <c r="I23" s="6">
-        <v>22</v>
+      <c r="C23" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="D23" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="E23" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="F23" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="G23" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="H23" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="I23" s="11" t="s">
+        <v>106</v>
       </c>
       <c r="J23" s="6" t="s">
         <v>12</v>
@@ -1240,26 +1273,26 @@
       <c r="B27" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C27" s="6">
-        <v>172</v>
-      </c>
-      <c r="D27" s="6">
-        <v>65</v>
-      </c>
-      <c r="E27" s="6">
-        <v>35.299999999999997</v>
-      </c>
-      <c r="F27" s="6">
-        <v>90</v>
-      </c>
-      <c r="G27" s="6">
-        <v>120</v>
-      </c>
-      <c r="H27" s="6">
-        <v>80</v>
-      </c>
-      <c r="I27" s="6">
-        <v>22</v>
+      <c r="C27" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="D27" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="E27" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="F27" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="G27" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="H27" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="I27" s="11" t="s">
+        <v>106</v>
       </c>
       <c r="J27" s="6" t="s">
         <v>12</v>
@@ -1301,8 +1334,8 @@
       <c r="C31" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="D31" s="6">
-        <v>30</v>
+      <c r="D31" s="11" t="s">
+        <v>98</v>
       </c>
       <c r="E31" s="6" t="s">
         <v>92</v>
@@ -1321,8 +1354,8 @@
       <c r="C32" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="D32" s="6">
-        <v>60</v>
+      <c r="D32" s="11" t="s">
+        <v>107</v>
       </c>
       <c r="E32" s="6" t="s">
         <v>93</v>
@@ -1341,8 +1374,8 @@
       <c r="C33" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="D33" s="6">
-        <v>90</v>
+      <c r="D33" s="11" t="s">
+        <v>103</v>
       </c>
       <c r="E33" s="6" t="s">
         <v>97</v>
@@ -1387,8 +1420,8 @@
       <c r="C37" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="D37" s="6">
-        <v>30</v>
+      <c r="D37" s="11" t="s">
+        <v>98</v>
       </c>
       <c r="E37" s="6" t="s">
         <v>92</v>
@@ -1407,8 +1440,8 @@
       <c r="C38" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="D38" s="6">
-        <v>60</v>
+      <c r="D38" s="11" t="s">
+        <v>107</v>
       </c>
       <c r="E38" s="6" t="s">
         <v>93</v>
@@ -1427,8 +1460,8 @@
       <c r="C39" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="D39" s="6">
-        <v>90</v>
+      <c r="D39" s="11" t="s">
+        <v>103</v>
       </c>
       <c r="E39" s="6" t="s">
         <v>97</v>
@@ -2016,11 +2049,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="A2:A11"/>
-    <mergeCell ref="A12:A19"/>
-    <mergeCell ref="C12:C19"/>
-    <mergeCell ref="A20:A27"/>
-    <mergeCell ref="C20:C27"/>
     <mergeCell ref="A61:A67"/>
     <mergeCell ref="C61:C67"/>
     <mergeCell ref="B2:B11"/>
@@ -2037,6 +2065,11 @@
     <mergeCell ref="A49:A60"/>
     <mergeCell ref="C49:C60"/>
     <mergeCell ref="C2:C11"/>
+    <mergeCell ref="A2:A11"/>
+    <mergeCell ref="A12:A19"/>
+    <mergeCell ref="C12:C19"/>
+    <mergeCell ref="A20:A27"/>
+    <mergeCell ref="C20:C27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>